<commit_message>
final evaluation data part 2
</commit_message>
<xml_diff>
--- a/aexpy/aexpy_evaluation_sklearn_0242_121.xlsx
+++ b/aexpy/aexpy_evaluation_sklearn_0242_121.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\BA\Library-Analyzer\aexpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F54FB-BB6D-4A2D-816C-0F2036925684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7583E0-1DD0-40E1-92BC-88C2C54B5DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{F2E66421-E238-4AFD-86C6-8E2F37411972}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2E66421-E238-4AFD-86C6-8E2F37411972}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4916" uniqueCount="1626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4924" uniqueCount="1634">
   <si>
     <t>sklearn.cluster._agglomerative.FeatureAgglomeration.fit</t>
   </si>
@@ -4914,6 +4914,30 @@
   </si>
   <si>
     <t>scikit-learn/sklearn.linear_model._stochastic_gradient/SGDClassifier/predict_proba remvoed @property</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>sek</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>ges</t>
+  </si>
+  <si>
+    <t>evaluating</t>
+  </si>
+  <si>
+    <t>reporting</t>
+  </si>
+  <si>
+    <t>differing</t>
   </si>
 </sst>
 </file>
@@ -4988,19 +5012,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5316,10 +5340,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6B4D18-7A72-424B-BC18-3449F54859C0}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B12:H353"/>
+  <dimension ref="B12:H361"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C358" sqref="C358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13261,7 +13285,7 @@
       </c>
     </row>
     <row r="346" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B346" s="5" t="s">
+      <c r="B346" s="8" t="s">
         <v>1593</v>
       </c>
       <c r="C346" s="4" t="s">
@@ -13269,25 +13293,25 @@
       </c>
     </row>
     <row r="347" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B347" s="5"/>
+      <c r="B347" s="8"/>
       <c r="C347" s="4" t="s">
         <v>1589</v>
       </c>
     </row>
     <row r="348" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B348" s="5"/>
+      <c r="B348" s="8"/>
       <c r="C348" s="4" t="s">
         <v>1590</v>
       </c>
     </row>
     <row r="349" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B349" s="5"/>
+      <c r="B349" s="8"/>
       <c r="C349" s="4" t="s">
         <v>1591</v>
       </c>
     </row>
     <row r="350" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B350" s="5"/>
+      <c r="B350" s="8"/>
       <c r="C350" s="4" t="s">
         <v>1592</v>
       </c>
@@ -13302,9 +13326,70 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="353" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C353" s="3" t="s">
         <v>1596</v>
+      </c>
+    </row>
+    <row r="356" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D356" s="9">
+        <v>1464.721918</v>
+      </c>
+      <c r="E356">
+        <f>D356/60</f>
+        <v>24.412031966666667</v>
+      </c>
+    </row>
+    <row r="357" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C357" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C358" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D358">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C359" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D359">
+        <f>19*60+19</f>
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="360" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C360" s="1" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D360" s="9">
+        <f>SUM(D356:D359)</f>
+        <v>2625.7219180000002</v>
+      </c>
+      <c r="E360" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="361" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D361">
+        <f>D360/60</f>
+        <v>43.762031966666669</v>
+      </c>
+      <c r="E361" t="s">
+        <v>1628</v>
       </c>
     </row>
   </sheetData>
@@ -13328,8 +13413,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B12:H357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B355" sqref="B355"/>
+    <sheetView topLeftCell="B38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C351" sqref="C351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21241,12 +21326,12 @@
       </c>
     </row>
     <row r="352" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C352" s="9" t="s">
+      <c r="C352" s="7" t="s">
         <v>1602</v>
       </c>
     </row>
     <row r="353" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C353" s="9" t="s">
+      <c r="C353" s="7" t="s">
         <v>1603</v>
       </c>
     </row>
@@ -21256,17 +21341,17 @@
       </c>
     </row>
     <row r="355" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C355" s="8" t="s">
+      <c r="C355" s="6" t="s">
         <v>1605</v>
       </c>
     </row>
     <row r="356" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C356" s="8" t="s">
+      <c r="C356" s="6" t="s">
         <v>1606</v>
       </c>
     </row>
     <row r="357" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C357" s="8" t="s">
+      <c r="C357" s="6" t="s">
         <v>1607</v>
       </c>
     </row>
@@ -21284,11 +21369,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69844BA6-B26D-4FD1-B7EB-6B9E847205CF}">
-  <sheetPr filterMode="1"/>
   <dimension ref="B12:H323"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="C321" sqref="C321:C322"/>
+    <sheetView topLeftCell="B300" workbookViewId="0">
+      <selection activeCell="C140" sqref="B139:C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21652,7 +21736,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>744</v>
       </c>
@@ -21675,7 +21759,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>93</v>
       </c>
@@ -21698,7 +21782,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>93</v>
       </c>
@@ -21721,7 +21805,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>81</v>
       </c>
@@ -21747,7 +21831,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>44</v>
       </c>
@@ -21773,7 +21857,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>44</v>
       </c>
@@ -21799,7 +21883,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>44</v>
       </c>
@@ -21825,7 +21909,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>44</v>
       </c>
@@ -21851,7 +21935,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>44</v>
       </c>
@@ -21877,7 +21961,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>44</v>
       </c>
@@ -21903,7 +21987,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>44</v>
       </c>
@@ -21929,7 +22013,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>44</v>
       </c>
@@ -21955,7 +22039,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>44</v>
       </c>
@@ -21978,7 +22062,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -22004,7 +22088,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -22030,7 +22114,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>44</v>
       </c>
@@ -22056,7 +22140,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>44</v>
       </c>
@@ -22082,7 +22166,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>42</v>
       </c>
@@ -22327,7 +22411,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="59" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>36</v>
       </c>
@@ -22350,7 +22434,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="60" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>36</v>
       </c>
@@ -22373,7 +22457,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="61" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>36</v>
       </c>
@@ -22396,7 +22480,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="62" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>36</v>
       </c>
@@ -22419,7 +22503,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>402</v>
       </c>
@@ -22442,7 +22526,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="64" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>36</v>
       </c>
@@ -22468,7 +22552,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="65" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>36</v>
       </c>
@@ -22494,7 +22578,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="66" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>36</v>
       </c>
@@ -22520,7 +22604,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="67" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>36</v>
       </c>
@@ -22546,7 +22630,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="68" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>36</v>
       </c>
@@ -22569,7 +22653,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="69" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>36</v>
       </c>
@@ -22592,7 +22676,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="70" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>744</v>
       </c>
@@ -22615,7 +22699,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="71" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>744</v>
       </c>
@@ -22638,7 +22722,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="72" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>69</v>
       </c>
@@ -22661,7 +22745,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="73" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>69</v>
       </c>
@@ -22684,7 +22768,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="74" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>69</v>
       </c>
@@ -22707,7 +22791,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="75" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>69</v>
       </c>
@@ -22730,7 +22814,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="76" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>69</v>
       </c>
@@ -22753,7 +22837,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="77" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>69</v>
       </c>
@@ -22776,7 +22860,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="78" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>69</v>
       </c>
@@ -22799,7 +22883,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="79" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>69</v>
       </c>
@@ -22822,7 +22906,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="80" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>69</v>
       </c>
@@ -22845,7 +22929,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="81" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>73</v>
       </c>
@@ -22868,7 +22952,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="82" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>73</v>
       </c>
@@ -22891,7 +22975,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="83" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>73</v>
       </c>
@@ -22914,7 +22998,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="84" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>73</v>
       </c>
@@ -22937,7 +23021,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="85" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>73</v>
       </c>
@@ -22960,7 +23044,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="86" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>73</v>
       </c>
@@ -22983,7 +23067,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="87" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>73</v>
       </c>
@@ -23006,7 +23090,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="88" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>73</v>
       </c>
@@ -23029,7 +23113,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="89" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>73</v>
       </c>
@@ -23052,7 +23136,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="90" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>73</v>
       </c>
@@ -23075,7 +23159,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="91" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>81</v>
       </c>
@@ -23101,7 +23185,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="92" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>81</v>
       </c>
@@ -23127,7 +23211,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="93" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>81</v>
       </c>
@@ -23153,7 +23237,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="94" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>81</v>
       </c>
@@ -23179,7 +23263,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="95" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>81</v>
       </c>
@@ -23205,7 +23289,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="96" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>81</v>
       </c>
@@ -23231,7 +23315,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>81</v>
       </c>
@@ -23257,7 +23341,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="98" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>81</v>
       </c>
@@ -23283,7 +23367,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>81</v>
       </c>
@@ -23309,7 +23393,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="100" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>93</v>
       </c>
@@ -23332,7 +23416,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="101" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>93</v>
       </c>
@@ -23355,7 +23439,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="102" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>93</v>
       </c>
@@ -23378,7 +23462,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="103" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>93</v>
       </c>
@@ -23401,7 +23485,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="104" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>93</v>
       </c>
@@ -23424,7 +23508,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="105" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>81</v>
       </c>
@@ -23450,7 +23534,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="106" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>81</v>
       </c>
@@ -23476,7 +23560,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="107" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>81</v>
       </c>
@@ -23502,7 +23586,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="108" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>81</v>
       </c>
@@ -23528,7 +23612,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="109" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>81</v>
       </c>
@@ -23554,7 +23638,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="110" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>81</v>
       </c>
@@ -23580,7 +23664,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="111" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>81</v>
       </c>
@@ -23606,7 +23690,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="112" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>81</v>
       </c>
@@ -23632,7 +23716,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="113" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>81</v>
       </c>
@@ -23658,7 +23742,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="114" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>81</v>
       </c>
@@ -23684,7 +23768,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="115" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>81</v>
       </c>
@@ -23710,7 +23794,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="116" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>81</v>
       </c>
@@ -23736,7 +23820,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="117" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>81</v>
       </c>
@@ -23762,7 +23846,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="118" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>81</v>
       </c>
@@ -23788,7 +23872,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="119" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>81</v>
       </c>
@@ -23814,7 +23898,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="120" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>81</v>
       </c>
@@ -23840,7 +23924,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="121" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>81</v>
       </c>
@@ -23866,7 +23950,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="122" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -23892,7 +23976,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="123" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>120</v>
       </c>
@@ -23918,7 +24002,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="124" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>120</v>
       </c>
@@ -23944,7 +24028,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="125" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>120</v>
       </c>
@@ -23970,7 +24054,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="126" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>120</v>
       </c>
@@ -23996,7 +24080,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="127" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>44</v>
       </c>
@@ -24022,7 +24106,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="128" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>44</v>
       </c>
@@ -24048,7 +24132,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="129" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>133</v>
       </c>
@@ -24071,7 +24155,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="130" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>133</v>
       </c>
@@ -24094,7 +24178,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="131" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>133</v>
       </c>
@@ -24117,7 +24201,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="132" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>133</v>
       </c>
@@ -24140,7 +24224,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="133" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>133</v>
       </c>
@@ -24163,7 +24247,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="134" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>852</v>
       </c>
@@ -24189,7 +24273,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="135" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>854</v>
       </c>
@@ -24215,7 +24299,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="136" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>133</v>
       </c>
@@ -24238,7 +24322,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="137" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>854</v>
       </c>
@@ -24264,7 +24348,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="138" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>42</v>
       </c>
@@ -24290,7 +24374,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="139" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>42</v>
       </c>
@@ -24316,7 +24400,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="140" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>42</v>
       </c>
@@ -24342,7 +24426,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="141" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>133</v>
       </c>
@@ -24365,7 +24449,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="142" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>133</v>
       </c>
@@ -24388,7 +24472,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="143" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>133</v>
       </c>
@@ -24411,7 +24495,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="144" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>133</v>
       </c>
@@ -24434,7 +24518,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="145" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>854</v>
       </c>
@@ -24460,7 +24544,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="146" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>854</v>
       </c>
@@ -24486,7 +24570,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="147" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>133</v>
       </c>
@@ -24509,7 +24593,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="148" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>133</v>
       </c>
@@ -24532,7 +24616,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="149" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>133</v>
       </c>
@@ -24578,7 +24662,7 @@
         <v>+</v>
       </c>
     </row>
-    <row r="151" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>149</v>
       </c>
@@ -24601,7 +24685,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="152" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>149</v>
       </c>
@@ -24647,7 +24731,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="154" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>149</v>
       </c>
@@ -24716,7 +24800,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="157" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>149</v>
       </c>
@@ -24739,7 +24823,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="158" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>149</v>
       </c>
@@ -24762,7 +24846,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="159" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>149</v>
       </c>
@@ -24785,7 +24869,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="160" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>149</v>
       </c>
@@ -24808,7 +24892,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="161" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>149</v>
       </c>
@@ -24831,7 +24915,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="162" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>149</v>
       </c>
@@ -24854,7 +24938,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="163" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>149</v>
       </c>
@@ -24877,7 +24961,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="164" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>149</v>
       </c>
@@ -24900,7 +24984,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="165" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>149</v>
       </c>
@@ -24923,7 +25007,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="166" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>184</v>
       </c>
@@ -24946,7 +25030,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="167" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>184</v>
       </c>
@@ -24969,7 +25053,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="168" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>184</v>
       </c>
@@ -24992,7 +25076,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="169" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>184</v>
       </c>
@@ -25015,7 +25099,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="170" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>184</v>
       </c>
@@ -25038,7 +25122,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="171" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>184</v>
       </c>
@@ -25061,7 +25145,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="172" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>184</v>
       </c>
@@ -25084,7 +25168,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="173" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>184</v>
       </c>
@@ -25107,7 +25191,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="174" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>184</v>
       </c>
@@ -25130,7 +25214,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="175" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>184</v>
       </c>
@@ -25153,7 +25237,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="176" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>184</v>
       </c>
@@ -25176,7 +25260,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="177" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>184</v>
       </c>
@@ -25199,7 +25283,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="178" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>184</v>
       </c>
@@ -25222,7 +25306,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="179" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>184</v>
       </c>
@@ -25245,7 +25329,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="180" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>224</v>
       </c>
@@ -25268,7 +25352,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="181" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>224</v>
       </c>
@@ -25291,7 +25375,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="182" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>224</v>
       </c>
@@ -25314,7 +25398,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="183" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>224</v>
       </c>
@@ -25337,7 +25421,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="184" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>224</v>
       </c>
@@ -25360,7 +25444,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="185" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>229</v>
       </c>
@@ -25386,7 +25470,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="186" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>229</v>
       </c>
@@ -25412,7 +25496,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="187" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>229</v>
       </c>
@@ -25438,7 +25522,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="188" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>229</v>
       </c>
@@ -25464,7 +25548,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="189" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>229</v>
       </c>
@@ -25490,7 +25574,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="190" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>229</v>
       </c>
@@ -25516,7 +25600,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="191" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>229</v>
       </c>
@@ -25542,7 +25626,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="192" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>229</v>
       </c>
@@ -25568,7 +25652,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="193" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>229</v>
       </c>
@@ -25594,7 +25678,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="194" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>229</v>
       </c>
@@ -25620,7 +25704,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="195" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>229</v>
       </c>
@@ -25646,7 +25730,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="196" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>229</v>
       </c>
@@ -25672,7 +25756,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="197" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>229</v>
       </c>
@@ -25698,7 +25782,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="198" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>229</v>
       </c>
@@ -25724,7 +25808,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="199" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>229</v>
       </c>
@@ -25750,7 +25834,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="200" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>229</v>
       </c>
@@ -25776,7 +25860,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="201" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>229</v>
       </c>
@@ -25802,7 +25886,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="202" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>229</v>
       </c>
@@ -25828,7 +25912,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="203" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>229</v>
       </c>
@@ -25854,7 +25938,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="204" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>229</v>
       </c>
@@ -25880,7 +25964,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="205" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>229</v>
       </c>
@@ -25906,7 +25990,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="206" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>229</v>
       </c>
@@ -25932,7 +26016,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="207" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>273</v>
       </c>
@@ -25955,7 +26039,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="208" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>278</v>
       </c>
@@ -25978,7 +26062,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="209" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>278</v>
       </c>
@@ -26001,7 +26085,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="210" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>278</v>
       </c>
@@ -26024,7 +26108,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="211" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>278</v>
       </c>
@@ -26047,7 +26131,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="212" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>278</v>
       </c>
@@ -26070,7 +26154,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="213" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>278</v>
       </c>
@@ -26093,7 +26177,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="214" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>278</v>
       </c>
@@ -26116,7 +26200,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="215" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>278</v>
       </c>
@@ -26139,7 +26223,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="216" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>278</v>
       </c>
@@ -26162,7 +26246,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="217" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>278</v>
       </c>
@@ -26185,7 +26269,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="218" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>278</v>
       </c>
@@ -26208,7 +26292,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="219" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>278</v>
       </c>
@@ -26231,7 +26315,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="220" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>278</v>
       </c>
@@ -26254,7 +26338,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="221" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>278</v>
       </c>
@@ -26277,7 +26361,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="222" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>278</v>
       </c>
@@ -26300,7 +26384,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="223" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>278</v>
       </c>
@@ -26323,7 +26407,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="224" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>278</v>
       </c>
@@ -26346,7 +26430,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="225" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>278</v>
       </c>
@@ -26369,7 +26453,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="226" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>278</v>
       </c>
@@ -26392,7 +26476,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="227" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>278</v>
       </c>
@@ -26415,7 +26499,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="228" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>278</v>
       </c>
@@ -26438,7 +26522,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="229" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>278</v>
       </c>
@@ -26461,7 +26545,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="230" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>278</v>
       </c>
@@ -26484,7 +26568,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="231" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>278</v>
       </c>
@@ -26507,7 +26591,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="232" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
         <v>278</v>
       </c>
@@ -26530,7 +26614,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="233" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>278</v>
       </c>
@@ -26553,7 +26637,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="234" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>278</v>
       </c>
@@ -26576,7 +26660,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="235" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>278</v>
       </c>
@@ -26599,7 +26683,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="236" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>278</v>
       </c>
@@ -26622,7 +26706,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="237" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>278</v>
       </c>
@@ -26645,7 +26729,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="238" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>278</v>
       </c>
@@ -26668,7 +26752,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="239" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
         <v>278</v>
       </c>
@@ -26691,7 +26775,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="240" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
         <v>278</v>
       </c>
@@ -26714,7 +26798,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="241" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>278</v>
       </c>
@@ -26737,7 +26821,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="242" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>278</v>
       </c>
@@ -26760,7 +26844,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="243" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>278</v>
       </c>
@@ -26783,7 +26867,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="244" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>229</v>
       </c>
@@ -26809,7 +26893,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="245" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>229</v>
       </c>
@@ -26835,7 +26919,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="246" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>229</v>
       </c>
@@ -26861,7 +26945,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="247" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>229</v>
       </c>
@@ -26887,7 +26971,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="248" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>229</v>
       </c>
@@ -26913,7 +26997,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="249" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>229</v>
       </c>
@@ -26939,7 +27023,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="250" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>229</v>
       </c>
@@ -26965,7 +27049,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="251" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>229</v>
       </c>
@@ -26991,7 +27075,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="252" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>229</v>
       </c>
@@ -27017,7 +27101,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="253" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>229</v>
       </c>
@@ -27043,7 +27127,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="254" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
         <v>229</v>
       </c>
@@ -27069,7 +27153,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="255" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
         <v>229</v>
       </c>
@@ -27095,7 +27179,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="256" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
         <v>229</v>
       </c>
@@ -27121,7 +27205,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="257" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
         <v>229</v>
       </c>
@@ -27147,7 +27231,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="258" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
         <v>229</v>
       </c>
@@ -27173,7 +27257,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="259" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
         <v>229</v>
       </c>
@@ -27199,7 +27283,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="260" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
         <v>229</v>
       </c>
@@ -27225,7 +27309,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="261" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
         <v>229</v>
       </c>
@@ -27251,7 +27335,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="262" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
         <v>229</v>
       </c>
@@ -27277,7 +27361,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="263" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
         <v>229</v>
       </c>
@@ -27303,7 +27387,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="264" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
         <v>229</v>
       </c>
@@ -27329,7 +27413,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="265" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
         <v>229</v>
       </c>
@@ -27355,7 +27439,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="266" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
         <v>229</v>
       </c>
@@ -27381,7 +27465,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="267" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
         <v>229</v>
       </c>
@@ -27407,7 +27491,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="268" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
         <v>229</v>
       </c>
@@ -27433,7 +27517,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="269" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
         <v>229</v>
       </c>
@@ -27459,7 +27543,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="270" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
         <v>229</v>
       </c>
@@ -27485,7 +27569,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="271" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
         <v>229</v>
       </c>
@@ -27511,7 +27595,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="272" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
         <v>229</v>
       </c>
@@ -27537,7 +27621,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="273" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
         <v>229</v>
       </c>
@@ -27563,7 +27647,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="274" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
         <v>229</v>
       </c>
@@ -27589,7 +27673,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="275" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
         <v>229</v>
       </c>
@@ -27615,7 +27699,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="276" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
         <v>229</v>
       </c>
@@ -27641,7 +27725,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="277" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
         <v>229</v>
       </c>
@@ -27667,7 +27751,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="278" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
         <v>229</v>
       </c>
@@ -27693,7 +27777,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="279" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
         <v>229</v>
       </c>
@@ -27719,7 +27803,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="280" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
         <v>229</v>
       </c>
@@ -27745,7 +27829,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="281" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
         <v>229</v>
       </c>
@@ -27771,7 +27855,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="282" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
         <v>229</v>
       </c>
@@ -27797,7 +27881,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="283" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
         <v>229</v>
       </c>
@@ -27823,7 +27907,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="284" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
         <v>229</v>
       </c>
@@ -27849,7 +27933,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="285" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
         <v>229</v>
       </c>
@@ -27875,7 +27959,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="286" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
         <v>229</v>
       </c>
@@ -27901,7 +27985,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="287" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
         <v>229</v>
       </c>
@@ -27927,7 +28011,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="288" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
         <v>229</v>
       </c>
@@ -27953,7 +28037,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="289" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
         <v>229</v>
       </c>
@@ -27979,7 +28063,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="290" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
         <v>229</v>
       </c>
@@ -28005,7 +28089,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="291" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
         <v>229</v>
       </c>
@@ -28031,7 +28115,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="292" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>229</v>
       </c>
@@ -28057,7 +28141,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="293" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
         <v>1030</v>
       </c>
@@ -28077,7 +28161,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="294" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
         <v>1031</v>
       </c>
@@ -28097,7 +28181,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="295" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
         <v>377</v>
       </c>
@@ -28123,7 +28207,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="296" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
         <v>377</v>
       </c>
@@ -28149,7 +28233,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="297" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
         <v>377</v>
       </c>
@@ -28175,7 +28259,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="298" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
         <v>377</v>
       </c>
@@ -28201,7 +28285,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="299" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
         <v>377</v>
       </c>
@@ -28227,7 +28311,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="300" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
         <v>377</v>
       </c>
@@ -28253,7 +28337,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="301" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
         <v>377</v>
       </c>
@@ -28279,7 +28363,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="302" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
         <v>377</v>
       </c>
@@ -28305,7 +28389,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="303" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
         <v>377</v>
       </c>
@@ -28331,7 +28415,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="304" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
         <v>377</v>
       </c>
@@ -28357,7 +28441,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="305" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
         <v>377</v>
       </c>
@@ -28383,7 +28467,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="306" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
         <v>377</v>
       </c>
@@ -28409,7 +28493,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="307" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
         <v>377</v>
       </c>
@@ -28432,7 +28516,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="308" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
         <v>1048</v>
       </c>
@@ -28452,7 +28536,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="309" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
         <v>377</v>
       </c>
@@ -28478,7 +28562,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="310" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
         <v>377</v>
       </c>
@@ -28504,7 +28588,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="311" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
         <v>377</v>
       </c>
@@ -28530,7 +28614,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="312" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
         <v>377</v>
       </c>
@@ -28556,7 +28640,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="313" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
         <v>377</v>
       </c>
@@ -28588,43 +28672,37 @@
       </c>
     </row>
     <row r="318" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C318" s="7" t="s">
+      <c r="C318" t="s">
         <v>1609</v>
       </c>
     </row>
     <row r="319" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C319" s="7" t="s">
+      <c r="C319" t="s">
         <v>1610</v>
       </c>
     </row>
     <row r="320" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C320" s="7" t="s">
+      <c r="C320" t="s">
         <v>1612</v>
       </c>
     </row>
     <row r="321" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C321" s="9" t="s">
+      <c r="C321" s="7" t="s">
         <v>1613</v>
       </c>
     </row>
     <row r="322" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C322" s="9" t="s">
+      <c r="C322" s="7" t="s">
         <v>1614</v>
       </c>
     </row>
     <row r="323" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C323" s="6" t="s">
+      <c r="C323" s="5" t="s">
         <v>1615</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B19:H313" xr:uid="{69844BA6-B26D-4FD1-B7EB-6B9E847205CF}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="+"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B19:H313" xr:uid="{69844BA6-B26D-4FD1-B7EB-6B9E847205CF}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -28635,7 +28713,7 @@
   <dimension ref="B12:H483"/>
   <sheetViews>
     <sheetView topLeftCell="B57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C482" sqref="C482:C483"/>
+      <selection activeCell="C57" sqref="B57:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39559,32 +39637,32 @@
       </c>
     </row>
     <row r="472" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C472" s="9" t="s">
+      <c r="C472" s="7" t="s">
         <v>1616</v>
       </c>
     </row>
     <row r="473" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C473" s="9" t="s">
+      <c r="C473" s="7" t="s">
         <v>1616</v>
       </c>
     </row>
     <row r="474" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C474" s="9" t="s">
+      <c r="C474" s="7" t="s">
         <v>1617</v>
       </c>
     </row>
     <row r="475" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C475" s="7" t="s">
+      <c r="C475" t="s">
         <v>1618</v>
       </c>
     </row>
     <row r="476" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C476" s="7" t="s">
+      <c r="C476" t="s">
         <v>1619</v>
       </c>
     </row>
     <row r="477" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C477" s="7" t="s">
+      <c r="C477" t="s">
         <v>1620</v>
       </c>
     </row>
@@ -39594,27 +39672,27 @@
       </c>
     </row>
     <row r="479" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C479" s="7" t="s">
+      <c r="C479" t="s">
         <v>1621</v>
       </c>
     </row>
     <row r="480" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C480" s="7" t="s">
+      <c r="C480" t="s">
         <v>1622</v>
       </c>
     </row>
     <row r="481" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C481" s="9" t="s">
+      <c r="C481" s="7" t="s">
         <v>1623</v>
       </c>
     </row>
     <row r="482" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C482" s="6" t="s">
+      <c r="C482" s="5" t="s">
         <v>1624</v>
       </c>
     </row>
     <row r="483" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C483" s="6" t="s">
+      <c r="C483" s="5" t="s">
         <v>1625</v>
       </c>
     </row>

</xml_diff>